<commit_message>
add remoting session and add flow chart
Co-Authored-By: ethanschafstall <7724486+ethanschafstall@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Doc/JNLTRAV/Journal-de-Travail_Nardou-Thomas.xlsx
+++ b/Doc/JNLTRAV/Journal-de-Travail_Nardou-Thomas.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -85,9 +85,6 @@
     <t>heures</t>
   </si>
   <si>
-    <t>Nom Prénom</t>
-  </si>
-  <si>
     <t>Date:</t>
   </si>
   <si>
@@ -104,6 +101,15 @@
   </si>
   <si>
     <t>Mettre en place le réseau interne</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Avec Ethan on a fais le digramme de flux </t>
+  </si>
+  <si>
+    <t>Nardou Thomas</t>
+  </si>
+  <si>
+    <t>J'ai fais la connection entre les PC</t>
   </si>
 </sst>
 </file>
@@ -555,7 +561,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
+      <selection pane="bottomLeft" activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -585,14 +591,14 @@
     </row>
     <row r="2" spans="1:14" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B2" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F2" s="12" t="s">
         <v>8</v>
@@ -619,16 +625,16 @@
       </c>
       <c r="C3" s="22">
         <f>SUM(C5:C521)</f>
-        <v>7.8472222222222221E-2</v>
+        <v>0.1111111111111111</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>14</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F3" s="13">
-        <v>44927</v>
+        <v>45259</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -666,7 +672,7 @@
         <v>11</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F6" s="11"/>
     </row>
@@ -685,7 +691,7 @@
         <v>11</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F7" s="11"/>
     </row>
@@ -704,30 +710,45 @@
         <v>11</v>
       </c>
       <c r="E8" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8" s="11"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="15">
+        <v>49</v>
+      </c>
+      <c r="B9" s="9">
+        <v>45266</v>
+      </c>
+      <c r="C9" s="10">
+        <v>2.361111111111111E-2</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="F8" s="11"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="str">
-        <f>IF(ISBLANK(B9),"",_xlfn.ISOWEEKNUM(Table2[[#This Row],[Jour]]))</f>
-        <v/>
-      </c>
-      <c r="B9" s="9"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
       <c r="F9" s="11"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="15" t="str">
+      <c r="A10" s="15">
         <f>IF(ISBLANK(B10),"",_xlfn.ISOWEEKNUM(Table2[[#This Row],[Jour]]))</f>
-        <v/>
-      </c>
-      <c r="B10" s="9"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
+        <v>49</v>
+      </c>
+      <c r="B10" s="9">
+        <v>45266</v>
+      </c>
+      <c r="C10" s="10">
+        <v>9.0277777777777787E-3</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>23</v>
+      </c>
       <c r="F10" s="11"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
@@ -6717,6 +6738,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
@@ -6725,15 +6755,6 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6756,6 +6777,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDECA689-F55E-43C8-8CEF-25DE741768EA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8EB0028C-89CE-4553-AB94-94DC6E832369}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -6770,12 +6799,4 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDECA689-F55E-43C8-8CEF-25DE741768EA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
add check if log exists system and update the JDT
</commit_message>
<xml_diff>
--- a/Doc/JNLTRAV/Journal-de-Travail_Nardou-Thomas.xlsx
+++ b/Doc/JNLTRAV/Journal-de-Travail_Nardou-Thomas.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="30">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -119,6 +119,15 @@
   </si>
   <si>
     <t>J'ai aidé Ethan à rgler son problème de connection entre ses deux VM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J'ai fusionné mon script avec celui d'ethan </t>
+  </si>
+  <si>
+    <t xml:space="preserve">J'ai paufine ma partie de code en reglant quelques bugs et en optimisant un peu mon code </t>
+  </si>
+  <si>
+    <t xml:space="preserve">J'ai regler quelque dernier petit bug et j'ai ajouté le système de verification si l'event log existe ou pas </t>
   </si>
 </sst>
 </file>
@@ -569,8 +578,8 @@
   <dimension ref="A1:N531"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E14" sqref="E14"/>
+      <pane ySplit="5" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -634,7 +643,7 @@
       </c>
       <c r="C3" s="22">
         <f>SUM(C5:C521)</f>
-        <v>0.14930555555555555</v>
+        <v>0.29791666666666661</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>14</v>
@@ -818,36 +827,60 @@
       <c r="F13" s="11"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="15" t="str">
+      <c r="A14" s="15">
         <f>IF(ISBLANK(B14),"",_xlfn.ISOWEEKNUM(Table2[[#This Row],[Jour]]))</f>
-        <v/>
-      </c>
-      <c r="B14" s="9"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
+        <v>50</v>
+      </c>
+      <c r="B14" s="9">
+        <v>45273</v>
+      </c>
+      <c r="C14" s="10">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>27</v>
+      </c>
       <c r="F14" s="11"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="15" t="str">
+      <c r="A15" s="15">
         <f>IF(ISBLANK(B15),"",_xlfn.ISOWEEKNUM(Table2[[#This Row],[Jour]]))</f>
-        <v/>
-      </c>
-      <c r="B15" s="9"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
+        <v>50</v>
+      </c>
+      <c r="B15" s="9">
+        <v>45273</v>
+      </c>
+      <c r="C15" s="10">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>28</v>
+      </c>
       <c r="F15" s="11"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="15" t="str">
+      <c r="A16" s="15">
         <f>IF(ISBLANK(B16),"",_xlfn.ISOWEEKNUM(Table2[[#This Row],[Jour]]))</f>
-        <v/>
-      </c>
-      <c r="B16" s="9"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
+        <v>51</v>
+      </c>
+      <c r="B16" s="9">
+        <v>45280</v>
+      </c>
+      <c r="C16" s="10">
+        <v>2.361111111111111E-2</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>29</v>
+      </c>
       <c r="F16" s="11"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -6771,15 +6804,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
@@ -6788,6 +6812,15 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6810,14 +6843,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDECA689-F55E-43C8-8CEF-25DE741768EA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8EB0028C-89CE-4553-AB94-94DC6E832369}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -6832,4 +6857,12 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDECA689-F55E-43C8-8CEF-25DE741768EA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
add the recommended point
</commit_message>
<xml_diff>
--- a/Doc/JNLTRAV/Journal-de-Travail_Nardou-Thomas.xlsx
+++ b/Doc/JNLTRAV/Journal-de-Travail_Nardou-Thomas.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="31">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -128,6 +128,9 @@
   </si>
   <si>
     <t xml:space="preserve">J'ai regler quelque dernier petit bug et j'ai ajouté le système de verification si l'event log existe ou pas </t>
+  </si>
+  <si>
+    <t>J'ai regler les point à améliorer discuté avec M. Meylan</t>
   </si>
 </sst>
 </file>
@@ -578,8 +581,8 @@
   <dimension ref="A1:N531"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E32" sqref="E32"/>
+      <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -643,7 +646,7 @@
       </c>
       <c r="C3" s="22">
         <f>SUM(C5:C521)</f>
-        <v>0.29791666666666661</v>
+        <v>0.33958333333333329</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>14</v>
@@ -884,14 +887,22 @@
       <c r="F16" s="11"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="15" t="str">
+      <c r="A17" s="15">
         <f>IF(ISBLANK(B17),"",_xlfn.ISOWEEKNUM(Table2[[#This Row],[Jour]]))</f>
-        <v/>
-      </c>
-      <c r="B17" s="9"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
+        <v>51</v>
+      </c>
+      <c r="B17" s="9">
+        <v>45280</v>
+      </c>
+      <c r="C17" s="10">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>30</v>
+      </c>
       <c r="F17" s="11"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -6804,6 +6815,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
@@ -6812,15 +6832,6 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6843,6 +6854,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDECA689-F55E-43C8-8CEF-25DE741768EA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8EB0028C-89CE-4553-AB94-94DC6E832369}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -6857,12 +6876,4 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDECA689-F55E-43C8-8CEF-25DE741768EA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
update script and the JTRAV
</commit_message>
<xml_diff>
--- a/Doc/JNLTRAV/Journal-de-Travail_Nardou-Thomas.xlsx
+++ b/Doc/JNLTRAV/Journal-de-Travail_Nardou-Thomas.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thonardou\Documents\GitHub\P-Script_Get-EventLog\Doc\JNLTRAV\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\P-Script_Get-EventLog\Doc\JNLTRAV\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38A43158-EE04-4511-A3A0-85B10E5CD251}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="-28920" yWindow="5115" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
@@ -17,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0">'Journal de travail'!$A$5:$F$5</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="34">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -138,11 +139,14 @@
   <si>
     <t>Finir les derniers ajustements du script</t>
   </si>
+  <si>
+    <t>J'ai commencé le powerpoint avec Ethan</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$]dd/mm/yyyy;@" x16r2:formatCode16="[$-en-CH,1]dd/mm/yyyy;@"/>
   </numFmts>
@@ -272,6 +276,50 @@
   </cellStyles>
   <dxfs count="13">
     <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
@@ -319,50 +367,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -377,22 +381,22 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A5:F531" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="A5:F531">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A5:F531" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+  <autoFilter ref="A5:F531" xr:uid="{00000000-0009-0000-0100-000002000000}">
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
     <filterColumn colId="4" hiddenButton="1"/>
     <filterColumn colId="5" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="6">
-    <tableColumn id="1" name="Semaine" dataDxfId="5">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Semaine" dataDxfId="10">
       <calculatedColumnFormula>IF(ISBLANK(B6),"",_xlfn.ISOWEEKNUM(Table2[[#This Row],[Jour]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Jour" dataDxfId="4"/>
-    <tableColumn id="3" name="Temps [h]" dataDxfId="3"/>
-    <tableColumn id="4" name="Type" dataDxfId="2"/>
-    <tableColumn id="5" name="Description" dataDxfId="1"/>
-    <tableColumn id="6" name="Remarques/problèmes" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Jour" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Temps [h]" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Type" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Description" dataDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Remarques/problèmes" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -582,13 +586,13 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:N531"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A94" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E123" sqref="E123"/>
+      <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -652,7 +656,7 @@
       </c>
       <c r="C3" s="22">
         <f>SUM(C5:C521)</f>
-        <v>0.375</v>
+        <v>0.40277777777777779</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>14</v>
@@ -950,14 +954,22 @@
       <c r="F19" s="11"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="15" t="str">
+      <c r="A20" s="15">
         <f>IF(ISBLANK(B20),"",_xlfn.ISOWEEKNUM(Table2[[#This Row],[Jour]]))</f>
-        <v/>
-      </c>
-      <c r="B20" s="9"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="11"/>
+        <v>1</v>
+      </c>
+      <c r="B20" s="9">
+        <v>45297</v>
+      </c>
+      <c r="C20" s="10">
+        <v>2.7777777777777776E-2</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>33</v>
+      </c>
       <c r="F20" s="11"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -6584,24 +6596,24 @@
   </sheetData>
   <sheetProtection insertHyperlinks="0" selectLockedCells="1" sort="0" autoFilter="0"/>
   <conditionalFormatting sqref="D6:D531">
-    <cfRule type="expression" dxfId="12" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="4" priority="1" stopIfTrue="1">
       <formula>$D6="Meeting"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="2">
+    <cfRule type="expression" dxfId="3" priority="2">
       <formula>$D6="Documentation"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="2" priority="3" stopIfTrue="1">
       <formula>$D6="Test"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="1" priority="4" stopIfTrue="1">
       <formula>$D6="Analyse"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="0" priority="6" stopIfTrue="1">
       <formula>$D6="Dévelopement"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D6:D531">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D6:D531" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>$I$2:$N$2</formula1>
     </dataValidation>
   </dataValidations>
@@ -6614,6 +6626,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D4F20F00DBE2EE49BE9523363A2DF18B" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="83ae57d85107fc73e8c281aedb059e49">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="99ffe1f3-7857-457f-add0-5bdef636f38d" xmlns:ns3="be0d3259-a7ce-4623-88ec-81594dfcbc1c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b000e6a26fbebedf4c24f086a5622afe" ns2:_="" ns3:_="">
     <xsd:import namespace="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
@@ -6836,27 +6868,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8EB0028C-89CE-4553-AB94-94DC6E832369}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDECA689-F55E-43C8-8CEF-25DE741768EA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{146BE2DA-6117-4657-9EA0-437EBB1E64B8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6873,29 +6910,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDECA689-F55E-43C8-8CEF-25DE741768EA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8EB0028C-89CE-4553-AB94-94DC6E832369}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>